<commit_message>
add new regex notes......
</commit_message>
<xml_diff>
--- a/Data Structures/Progress log.xlsx
+++ b/Data Structures/Progress log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tat97\WC_LC\Data Structures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{190B8BF6-2E64-45DB-98F5-2CE907EDE18A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2739EE2F-94FC-4627-BE8E-1AE7CEC3178D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14712" yWindow="252" windowWidth="15084" windowHeight="15756" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3636" yWindow="288" windowWidth="21000" windowHeight="15756" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="1" r:id="rId1"/>
@@ -640,6 +640,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>421341</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>833718</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>203427</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>2430678</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{45BAA1E5-4F87-F58B-B376-504AEA6B3D99}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11313459" y="8319247"/>
+          <a:ext cx="8316486" cy="4887007"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1042,7 +1091,7 @@
   <dimension ref="A2:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1172,5 +1221,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>